<commit_message>
pegando texto dinamico da tabela
</commit_message>
<xml_diff>
--- a/contatos.xlsx
+++ b/contatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared\Documents\Projetos\send-whats-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112A41A8-2988-4195-B01F-2FD66FAFF438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE83592F-91E9-4D74-AD1D-B20FCFEAD3E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{7FBE834C-6018-44EC-A58A-5A914A64134B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
   <si>
     <t>Nome</t>
   </si>
@@ -34,6 +34,23 @@
   </si>
   <si>
     <t>Jared</t>
+  </si>
+  <si>
+    <t>Ola, este é um teste de mensagem com 
+enter pulando linda, e com emojissss 📚📚
+e mais enters e linhas puladas e a proxima vai começar com emoji em 
+⏱️⏱️ olha sóoo, reloginhos agoraaaa, agora que ja tem mensagens estranhas e emojis estranhos vamos de
+emojis Comunssss 😀😀
+Ola, este é um teste de mensagem com 
+enter pulando linda, e com emojissss 📚📚
+e mais enters e linhas puladas e a proxima vai começar com emoji em 
+⏱️⏱️ olha sóoo, reloginhos agoraaaa, agora que ja tem mensagens estranhas e emojis estranhos vamos de
+emojis Comunssss 😀😀
+😂😁😂😊😔😰😕😉
+e ultima linha amém</t>
+  </si>
+  <si>
+    <t>Mensagem</t>
   </si>
 </sst>
 </file>
@@ -69,8 +86,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,105 +405,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF2F416-235C-4F2D-A5F9-B04932D2E7D1}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.85546875" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10">
         <v>61999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11">
         <v>61999999999</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>